<commit_message>
forgot password pin automation added and input time error in create activity is solved
</commit_message>
<xml_diff>
--- a/TestData/Create Activity page/tc37.xlsx
+++ b/TestData/Create Activity page/tc37.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohni\PycharmProjects\cchc_automation\TestData\Create Activity page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D65872E-4CB0-4D95-B5EB-D0E740CC0082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5CE732-186E-4983-8926-F1A67B6667BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>mohini@mistpl.com</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>C:\Users\mohni\Downloads\RecActivity app.mp4</t>
+  </si>
+  <si>
+    <t>Bhagwan@123</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,8 +445,8 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>12345</v>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="3">
         <v>45423</v>
@@ -464,8 +467,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{4ECD84E5-BDB9-44B3-8F50-46A2DEEFD994}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{C8316AB7-41E2-437C-B69D-F6E424435DD4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>